<commit_message>
200 LOC: added start/end for laws
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/laws-authorities.xlsx
+++ b/documentation-generator/vocab_csv/laws-authorities.xlsx
@@ -493,7 +493,7 @@
     <t>http://www.bfdi.bund.de/</t>
   </si>
   <si>
-    <t>legal-DE:BDSG,legal-eu:GDPR</t>
+    <t>legal-de:BDSG,legal-eu:GDPR</t>
   </si>
   <si>
     <t>DPA-DE-BB</t>
@@ -505,7 +505,7 @@
     <t>https://www.lda.brandenburg.de/</t>
   </si>
   <si>
-    <t>legal-DE:BDSG,legal-DE:BE-BbgDSG,legal-eu:GDPR</t>
+    <t>legal-de:BDSG,legal-de:BE-BbgDSG,legal-eu:GDPR</t>
   </si>
   <si>
     <t>DPA-DE-BE</t>
@@ -517,7 +517,7 @@
     <t>https://www.datenschutz-berlin.de/</t>
   </si>
   <si>
-    <t>legal-DE:BDSG,legal-DE:BE-BlnDSG,legal-eu:GDPR</t>
+    <t>legal-de:BDSG,legal-de:BE-BlnDSG,legal-eu:GDPR</t>
   </si>
   <si>
     <t>DPA-DE-BY-non-public</t>
@@ -529,7 +529,7 @@
     <t>https://www.lda.bayern.de/</t>
   </si>
   <si>
-    <t>legal-DE:BDSG,legal-DE:BY-BayDSG,legal-eu:GDPR</t>
+    <t>legal-de:BDSG,legal-de:BY-BayDSG,legal-eu:GDPR</t>
   </si>
   <si>
     <t>DPA-DE-BY-public</t>
@@ -550,7 +550,7 @@
     <t>https://www.datenschutz.bremen.de/</t>
   </si>
   <si>
-    <t>legal-DE:BDSG,legal-DE:HB-BremDSGVOAG,legal-eu:GDPR</t>
+    <t>legal-de:BDSG,legal-de:HB-BremDSGVOAG,legal-eu:GDPR</t>
   </si>
   <si>
     <t>DPA-DE-HE</t>
@@ -562,7 +562,7 @@
     <t>https://www.datenschutz.hessen.de/</t>
   </si>
   <si>
-    <t>legal-DE:BDSG,legal-DE:HE-HDISG,legal-eu:GDPR</t>
+    <t>legal-de:BDSG,legal-de:HE-HDISG,legal-eu:GDPR</t>
   </si>
   <si>
     <t>DPA-DE-HH</t>
@@ -574,7 +574,7 @@
     <t>https://www.datenschutz-hamburg.de/</t>
   </si>
   <si>
-    <t>legal-DE:BDSG,legal-DE:HH-HmbDSG,legal-eu:GDPR</t>
+    <t>legal-de:BDSG,legal-de:HH-HmbDSG,legal-eu:GDPR</t>
   </si>
   <si>
     <t>DPA-DE-MV</t>
@@ -586,7 +586,7 @@
     <t>https://www.datenschutz-mv.de/</t>
   </si>
   <si>
-    <t>legal-DE:BDSG,legal-DE:MV-DSG,legal-eu:GDPR</t>
+    <t>legal-de:BDSG,legal-de:MV-DSG,legal-eu:GDPR</t>
   </si>
   <si>
     <t>DPA-DE-NI</t>
@@ -598,7 +598,7 @@
     <t>https://www.lfd.niedersachsen.de/</t>
   </si>
   <si>
-    <t>legal-DE:BDSG,legal-DE:NI-NDSG,legal-eu:GDPR</t>
+    <t>legal-de:BDSG,legal-de:NI-NDSG,legal-eu:GDPR</t>
   </si>
   <si>
     <t>DPA-DE-NW</t>
@@ -610,7 +610,7 @@
     <t>https://www.ldi.nrw.de/</t>
   </si>
   <si>
-    <t>legal-DE:BDSG,legal-DE:NW-DSG,legal-eu:GDPR</t>
+    <t>legal-de:BDSG,legal-de:NW-DSG,legal-eu:GDPR</t>
   </si>
   <si>
     <t>DPA-DE-RP</t>
@@ -622,7 +622,7 @@
     <t>https://www.datenschutz.rlp.de/</t>
   </si>
   <si>
-    <t>legal-DE:BDSG,legal-DE:RP-LDSG,legal-eu:GDPR</t>
+    <t>legal-de:BDSG,legal-de:RP-LDSG,legal-eu:GDPR</t>
   </si>
   <si>
     <t>DPA-DE-SH</t>
@@ -634,7 +634,7 @@
     <t>https://www.datenschutzzentrum.de/</t>
   </si>
   <si>
-    <t>legal-DE:BDSG,legal-DE:SH-LDSG,legal-eu:GDPR</t>
+    <t>legal-de:BDSG,legal-de:SH-LDSG,legal-eu:GDPR</t>
   </si>
   <si>
     <t>DPA-DE-SL</t>
@@ -646,7 +646,7 @@
     <t>https://www.datenschutz.saarland.de/</t>
   </si>
   <si>
-    <t>legal-DE:BDSG,legal-DE:SL-SDSG,legal-eu:GDPR</t>
+    <t>legal-de:BDSG,legal-de:SL-SDSG,legal-eu:GDPR</t>
   </si>
   <si>
     <t>DPA-DE-SN</t>
@@ -658,7 +658,7 @@
     <t>https://www.saechsdsb.de/</t>
   </si>
   <si>
-    <t>legal-DE:BDSG,legal-DE:SN-SächsDSG,legal-eu:GDPR</t>
+    <t>legal-de:BDSG,legal-de:SN-SächsDSG,legal-eu:GDPR</t>
   </si>
   <si>
     <t>DPA-DE-ST</t>
@@ -670,7 +670,7 @@
     <t>https://datenschutz.sachsen-anhalt.de/</t>
   </si>
   <si>
-    <t>legal-DE:BDSG,legal-DE:LSA-DSG,legal-eu:GDPR</t>
+    <t>legal-de:BDSG,legal-de:LSA-DSG,legal-eu:GDPR</t>
   </si>
   <si>
     <t>DPA-DE-TH</t>
@@ -682,7 +682,7 @@
     <t>https://www.tlfdi.de/</t>
   </si>
   <si>
-    <t>legal-DE:BDSG,legal-DE:TH-ThürDSG,legal-eu:GDPR</t>
+    <t>legal-de:BDSG,legal-de:TH-ThürDSG,legal-eu:GDPR</t>
   </si>
   <si>
     <t>German Labels</t>

</xml_diff>